<commit_message>
fixed the address object in employer upload and same changes in template
</commit_message>
<xml_diff>
--- a/employerProfileUploadTemplate.xlsx
+++ b/employerProfileUploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hammertechcomau-my.sharepoint.com/personal/guy_accettura_hammertechglobal_com/Documents/Documents/Internal/PythonUploads/hammertech-worker-uploader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D23CD585-0892-410B-A590-57CE8AC642AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{D23CD585-0892-410B-A590-57CE8AC642AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F492921D-A735-4C81-ACAF-2DD92E094FCD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4236BBD2-939A-4B04-AD27-C929C2060649}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4236BBD2-939A-4B04-AD27-C929C2060649}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Business Name</t>
   </si>
@@ -44,12 +44,6 @@
     <t>ABN</t>
   </si>
   <si>
-    <t>Address Line 1</t>
-  </si>
-  <si>
-    <t>Address Line 2</t>
-  </si>
-  <si>
     <t>City / Suburb</t>
   </si>
   <si>
@@ -63,6 +57,9 @@
   </si>
   <si>
     <t>Internal Identifier</t>
+  </si>
+  <si>
+    <t>Street Address</t>
   </si>
 </sst>
 </file>
@@ -434,25 +431,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77308ABF-E46F-4C56-914F-B6520DCBA208}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,25 +457,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>